<commit_message>
Update ps values of some seeds
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_3_0/PrescaleTable/L1Menu_Collisions2022_v1_3_0-13.6TeV_2748b.xlsx
+++ b/development/L1Menu_Collisions2022_v1_3_0/PrescaleTable/L1Menu_Collisions2022_v1_3_0-13.6TeV_2748b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master 4/development/L1Menu_Collisions2022_v1_3_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6763DAC-55FF-D447-9AB8-9F18AD41ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FFB2D1-D84D-F449-A147-0E739EBE7161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20380" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20380" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2554,8 +2554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV404"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2961,28 +2961,28 @@
         <v>0</v>
       </c>
       <c r="D12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="E12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="F12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="G12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="H12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="I12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="J12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
       <c r="K12" s="5">
-        <v>1700</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3699,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F33" s="5">
         <v>4</v>
@@ -9194,7 +9194,7 @@
         <v>0</v>
       </c>
       <c r="E190" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F190" s="5">
         <v>1</v>
@@ -9229,7 +9229,7 @@
         <v>1</v>
       </c>
       <c r="E191" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F191" s="5">
         <v>1</v>

</xml_diff>